<commit_message>
Add tests: test_compare_file_names, test_compare_files_data
</commit_message>
<xml_diff>
--- a/tests/expected_data/ТЗ_ИНВЕСТИЦИИ_Кабельно-проводниковая продукция_Общее.xlsx
+++ b/tests/expected_data/ТЗ_ИНВЕСТИЦИИ_Кабельно-проводниковая продукция_Общее.xlsx
@@ -201,10 +201,10 @@
   </si>
   <si>
     <t>Поставка осуществляется путем отгрузок продукции автомобильным транспортом силами и за счет Поставщика до склада Грузополучателя по адресу:
-Исполнительный аппарат, 603005, г. Нижний Новгород, Алексеевская 10/16 БЦ "Лобачевский Плаза"
+Сормовская ТЭЦ, 603950, г. Нижний Новгород, ул. Коминтерна, д. 45
+Новогорьковская ТЭЦ, 607650, Нижегородская обл, г. Кстово, промзона
 Дзержинская ТЭЦ, 606000 Нижегородская область, г. Дзержинск, промзона
-Сормовская ТЭЦ, 603950, г. Нижний Новгород, ул. Коминтерна, д. 45
-Новогорьковская ТЭЦ, 607650, Нижегородская обл, г. Кстово, промзона</t>
+Исполнительный аппарат, 603005, г. Нижний Новгород, Алексеевская 10/16 БЦ "Лобачевский Плаза"</t>
   </si>
 </sst>
 </file>

</xml_diff>